<commit_message>
Optimize the backend architecture (Close #99)
</commit_message>
<xml_diff>
--- a/TestDataGeneration/FinalTestData.xlsx
+++ b/TestDataGeneration/FinalTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wenda\Desktop\Team Projects\备份\main\TestDataGeneration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wenda\Desktop\Team Projects\最新一次\main\TestDataGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5628EB-5593-4521-8C94-C00D249FC5BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8FB585-47C1-43F2-AF10-11B7C4C9FC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="1836" windowWidth="29040" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6828" yWindow="2652" windowWidth="23892" windowHeight="13608" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>